<commit_message>
Form Fill functionlity added Delete record from the grid functionality added.
</commit_message>
<xml_diff>
--- a/ConsoleApp1/TestData/Sample Test data.xlsx
+++ b/ConsoleApp1/TestData/Sample Test data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Demo1\Demo\ConsoleApp1\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A542A117-B419-4761-AC33-16FE3CB51261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DE8432-A9A5-4C5C-BFEA-BAD8A8DA9B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1262D413-3EE8-4B99-B800-C27A2A3ADF1F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{1262D413-3EE8-4B99-B800-C27A2A3ADF1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Patel" sheetId="2" r:id="rId1"/>
     <sheet name="Vijay" sheetId="1" r:id="rId2"/>
+    <sheet name="FormData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Sr no</t>
   </si>
@@ -48,16 +48,87 @@
   </si>
   <si>
     <t>Patel</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>DateOfBirthd</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Hobbies</t>
+  </si>
+  <si>
+    <t>PicturePath</t>
+  </si>
+  <si>
+    <t>CurrentAddress</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>patel@abc.com</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Sports;Reading</t>
+  </si>
+  <si>
+    <t>Stanza leaving</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>Panipat</t>
+  </si>
+  <si>
+    <t>01 Jan 1990</t>
+  </si>
+  <si>
+    <t>Picture.jpg</t>
+  </si>
+  <si>
+    <t>Maths;English;Computer Science</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,13 +151,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,7 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87488431-39B3-45DB-97C5-CF4A7F1A6F3E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -545,4 +620,109 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1793B31-66FF-481D-BA84-027B2576762A}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>1234567890</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{A93AEDE6-9AAF-492E-8A4D-BB2FB076AEC8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>